<commit_message>
Minor adjustments to templates (removing blank rows, adding header values).  Added new PartManufacturer template.
</commit_message>
<xml_diff>
--- a/Loading/Part/PartAdjustment.Template.xlsx
+++ b/Loading/Part/PartAdjustment.Template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Control</t>
   </si>
@@ -48,6 +48,30 @@
   </si>
   <si>
     <t>Unit Price</t>
+  </si>
+  <si>
+    <t>2091</t>
+  </si>
+  <si>
+    <t>380:2</t>
+  </si>
+  <si>
+    <t>380:5</t>
+  </si>
+  <si>
+    <t>380:7</t>
+  </si>
+  <si>
+    <t>381:2</t>
+  </si>
+  <si>
+    <t>381:4</t>
+  </si>
+  <si>
+    <t>381:6</t>
+  </si>
+  <si>
+    <t>381:8</t>
   </si>
 </sst>
 </file>
@@ -91,10 +115,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,11 +402,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -415,6 +440,32 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>